<commit_message>
Implementasi Interface pada pilihan jawaban.
</commit_message>
<xml_diff>
--- a/Burntdown Chart.xlsx
+++ b/Burntdown Chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Card</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Day2</t>
+  </si>
+  <si>
+    <t>Day3</t>
+  </si>
+  <si>
+    <t>Interface Penampilan Soal Pilihan</t>
   </si>
 </sst>
 </file>
@@ -113,6 +125,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -120,7 +135,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="id-ID"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -183,6 +198,9 @@
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -234,6 +252,9 @@
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -285,6 +306,9 @@
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -336,6 +360,9 @@
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -349,22 +376,22 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="79070336"/>
-        <c:axId val="79071872"/>
+        <c:axId val="251673872"/>
+        <c:axId val="251672696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79070336"/>
+        <c:axId val="251673872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79071872"/>
+        <c:crossAx val="251672696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -372,7 +399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79071872"/>
+        <c:axId val="251672696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -383,7 +410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79070336"/>
+        <c:crossAx val="251673872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -403,6 +430,1033 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0108705161854773E-2"/>
+          <c:y val="0.14393518518518519"/>
+          <c:w val="0.68788145303912807"/>
+          <c:h val="0.61498432487605714"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$24:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Interface Penampilan Soal Pilihan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pembukaan Slide</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Penyusunan soal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="251675048"/>
+        <c:axId val="251673088"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="251675048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="251673088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="251673088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="251675048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.77685463122710963"/>
+          <c:y val="0.14409667541557306"/>
+          <c:w val="0.17889608115295308"/>
+          <c:h val="0.59201443569553802"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,6 +1486,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -483,7 +1567,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,7 +1602,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -727,15 +1811,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -770,6 +1854,9 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -781,6 +1868,9 @@
       <c r="C4">
         <v>1</v>
       </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -792,6 +1882,9 @@
       <c r="C5">
         <v>2</v>
       </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -803,10 +1896,79 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementasi Interface Pada Pilgan
</commit_message>
<xml_diff>
--- a/Burntdown Chart.xlsx
+++ b/Burntdown Chart.xlsx
@@ -377,11 +377,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="251673872"/>
-        <c:axId val="251672696"/>
+        <c:axId val="243317496"/>
+        <c:axId val="243320632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="251673872"/>
+        <c:axId val="243317496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,7 +391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251672696"/>
+        <c:crossAx val="243320632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -399,7 +399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251672696"/>
+        <c:axId val="243320632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,7 +410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251673872"/>
+        <c:crossAx val="243317496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -561,7 +561,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,7 +624,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -687,7 +687,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,11 +703,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="251675048"/>
-        <c:axId val="251673088"/>
+        <c:axId val="243319848"/>
+        <c:axId val="243320240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="251675048"/>
+        <c:axId val="243319848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,7 +750,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251673088"/>
+        <c:crossAx val="243320240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -758,7 +758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251673088"/>
+        <c:axId val="243320240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +809,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251675048"/>
+        <c:crossAx val="243319848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1814,7 +1814,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
         <v>2</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1948,7 +1948,7 @@
         <v>3</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1962,7 +1962,7 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated some new things + Pergantian di soal nomor 10 pada QUestion.docx
</commit_message>
<xml_diff>
--- a/Burntdown Chart.xlsx
+++ b/Burntdown Chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Card</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Interface Penampilan Soal Pilihan</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Menambahkan SFX</t>
+  </si>
+  <si>
+    <t>Implementasikan Soal ke Dalam Slide</t>
+  </si>
+  <si>
+    <t>Menampilkan penjelasan dari jawaban</t>
   </si>
 </sst>
 </file>
@@ -376,12 +388,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243317496"/>
-        <c:axId val="243320632"/>
+        <c:axId val="84683392"/>
+        <c:axId val="84685184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243317496"/>
+        <c:axId val="84683392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,7 +404,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243320632"/>
+        <c:crossAx val="84685184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -399,7 +412,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243320632"/>
+        <c:axId val="84685184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,7 +423,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243317496"/>
+        <c:crossAx val="84683392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -702,12 +715,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243319848"/>
-        <c:axId val="243320240"/>
+        <c:axId val="84723968"/>
+        <c:axId val="84869120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243319848"/>
+        <c:axId val="84723968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,7 +764,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243320240"/>
+        <c:crossAx val="84869120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -758,7 +772,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243320240"/>
+        <c:axId val="84869120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243319848"/>
+        <c:crossAx val="84723968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -903,6 +917,252 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Menambahkan SFX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$35:$D$36</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$37:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Implementasikan Soal ke Dalam Slide</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$35:$D$36</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Menampilkan penjelasan dari jawaban</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$35:$D$36</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$39:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="84899328"/>
+        <c:axId val="84900864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="84899328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84900864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84900864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84899328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1521,6 +1781,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1567,7 +1857,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1602,7 +1892,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1811,10 +2101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,10 +2255,75 @@
         <v>1</v>
       </c>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>